<commit_message>
Created test bench for counter module
</commit_message>
<xml_diff>
--- a/Documentation/Test_Cases/Counter_Test_Cases.xlsx
+++ b/Documentation/Test_Cases/Counter_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\StopWatch_Verilog\git_repo\Time_Travelers_Verilog_Stopwatch\Documentation\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7AEC0A-AF7B-491D-8BDE-09F07536A302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27758117-3731-4D50-A977-CBFADE1F71A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,9 +686,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -697,21 +697,21 @@
         <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -720,13 +720,13 @@
         <v>53</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -743,7 +743,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>54</v>
@@ -751,13 +751,13 @@
       <c r="F4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -766,16 +766,16 @@
         <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1039,6 +1039,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1184,22 +1199,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099A5288-121E-4A14-A6B4-83046D76B9FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1215,21 +1232,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
counter test results created
</commit_message>
<xml_diff>
--- a/Documentation/Test_Cases/Counter_Test_Cases.xlsx
+++ b/Documentation/Test_Cases/Counter_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\StopWatch_Verilog\git_repo\Time_Travelers_Verilog_Stopwatch\Documentation\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27758117-3731-4D50-A977-CBFADE1F71A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6988D23-C450-4E6D-83C2-63A6F83F4F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -207,12 +207,6 @@
     <t>observe 'o_count' nibbles and compare to the respective 'o_bcdcount'</t>
   </si>
   <si>
-    <t>i_countenb' of every counter is connected to the flag output 'o_rolloverflag' of the previous counter</t>
-  </si>
-  <si>
-    <t>observe 'i_countenb' and compare to the respective 'o_rolloverflag'</t>
-  </si>
-  <si>
     <t>o_count'[3:0] = 'o_bcdcount0'</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>o_count'[23:20] = 'o_bcdcount5'</t>
   </si>
   <si>
-    <t>icountenb' of every subcounter = previous 'o_rolloverflag' except first one 'i_countenb' from trigger detection</t>
-  </si>
-  <si>
     <t>Check if 'o_bcdcount' is set to "0000" when 'i_reset_n' is set to 0</t>
   </si>
   <si>
@@ -262,6 +253,18 @@
   </si>
   <si>
     <t>set 'i_reset_n' to 1, increment 'o_count' then after 10 ns set 'i_reset_n' to 0</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>i_rtcclk' of every counter is connected to the flag output 'o_rolloverflag' of the previous counter</t>
+  </si>
+  <si>
+    <t>observe 'i_rtcclk' and compare to the respective 'o_rolloverflag'</t>
+  </si>
+  <si>
+    <t>i_rtcclk' of every subcounter = previous 'o_rolloverflag' except first one 'i_rtcclk' from trigger detection</t>
   </si>
 </sst>
 </file>
@@ -637,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,6 +711,12 @@
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -720,16 +729,22 @@
         <v>53</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -754,6 +769,12 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -777,6 +798,12 @@
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -800,8 +827,14 @@
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -812,16 +845,22 @@
         <v>53</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -844,7 +883,13 @@
         <v>47</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -858,7 +903,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>58</v>
@@ -867,7 +912,13 @@
         <v>47</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -881,7 +932,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>58</v>
@@ -890,7 +941,13 @@
         <v>47</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -904,7 +961,7 @@
         <v>53</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>58</v>
@@ -913,7 +970,13 @@
         <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -927,7 +990,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>58</v>
@@ -936,7 +999,13 @@
         <v>47</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -950,7 +1019,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>58</v>
@@ -959,7 +1028,13 @@
         <v>47</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -984,6 +1059,12 @@
       <c r="G14" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1007,8 +1088,14 @@
       <c r="G15" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1019,16 +1106,22 @@
         <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>51</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1039,21 +1132,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1199,24 +1277,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099A5288-121E-4A14-A6B4-83046D76B9FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1232,4 +1308,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding requirement tags to test case results
</commit_message>
<xml_diff>
--- a/Documentation/Test_Cases/Counter_Test_Cases.xlsx
+++ b/Documentation/Test_Cases/Counter_Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\StopWatch_Verilog\git_repo\Time_Travelers_Verilog_Stopwatch\Documentation\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6988D23-C450-4E6D-83C2-63A6F83F4F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5E5579-F71D-41EC-9DE8-AFB7637AC284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="80">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>i_rtcclk' of every subcounter = previous 'o_rolloverflag' except first one 'i_rtcclk' from trigger detection</t>
+  </si>
+  <si>
+    <t>2b20aa4</t>
   </si>
 </sst>
 </file>
@@ -640,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,6 +720,9 @@
       <c r="I2" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -746,6 +752,9 @@
       <c r="I3" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -775,6 +784,9 @@
       <c r="I4" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -804,6 +816,9 @@
       <c r="I5" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -833,6 +848,9 @@
       <c r="I6" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -862,6 +880,9 @@
       <c r="I7" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -891,6 +912,9 @@
       <c r="I8" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -920,6 +944,9 @@
       <c r="I9" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -949,6 +976,9 @@
       <c r="I10" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -978,6 +1008,9 @@
       <c r="I11" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1007,6 +1040,9 @@
       <c r="I12" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1036,6 +1072,9 @@
       <c r="I13" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J13" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1065,6 +1104,9 @@
       <c r="I14" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J14" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1094,6 +1136,9 @@
       <c r="I15" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="J15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1122,6 +1167,9 @@
       </c>
       <c r="I16" s="3" t="s">
         <v>75</v>
+      </c>
+      <c r="J16" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1278,18 +1326,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1311,18 +1359,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>